<commit_message>
Select + 1 var
Selecionado MemberKey
</commit_message>
<xml_diff>
--- a/Legenda dos dados.xlsx
+++ b/Legenda dos dados.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafae\Downloads\Udacity\UD_NDS_ProspeR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A0B7BC5-ED79-42A4-B1C6-8AA55090030D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF2289A5-F3DE-4372-8B41-D54960EF1F10}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="4575" windowWidth="20730" windowHeight="11310" xr2:uid="{05569AFF-E332-4AE5-ABAC-E9164803E6F8}"/>
+    <workbookView xWindow="-15480" yWindow="-120" windowWidth="15600" windowHeight="11310" xr2:uid="{05569AFF-E332-4AE5-ABAC-E9164803E6F8}"/>
   </bookViews>
   <sheets>
     <sheet name="Traduzido" sheetId="1" r:id="rId1"/>
@@ -1084,6 +1084,9 @@
       <colorFilter dxfId="0"/>
     </filterColumn>
   </autoFilter>
+  <sortState ref="A2:B82">
+    <sortCondition ref="A1:A82"/>
+  </sortState>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{EA51D860-C533-494E-8BD9-2036ECED9149}" name="Variável" dataDxfId="8"/>
     <tableColumn id="2" xr3:uid="{CFC57B81-AA85-44FD-8151-860766CCDBA0}" name="Descrição" dataDxfId="7"/>
@@ -1403,7 +1406,7 @@
   <dimension ref="A1:B82"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="A2:B82"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1422,50 +1425,50 @@
     </row>
     <row r="2" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>81</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>1</v>
+        <v>42</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>82</v>
+        <v>123</v>
       </c>
     </row>
     <row r="4" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>2</v>
+      <c r="A4" s="6" t="s">
+        <v>41</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>3</v>
+        <v>122</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>7</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>5</v>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>86</v>
+        <v>98</v>
       </c>
     </row>
     <row r="8" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -1476,596 +1479,596 @@
         <v>87</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>7</v>
+    <row r="9" spans="1:2" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>3</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>8</v>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>91</v>
+        <v>109</v>
       </c>
     </row>
     <row r="13" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B21" s="2" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+    <row r="22" spans="1:2" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B22" s="2" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="51" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
     </row>
     <row r="24" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="25" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>104</v>
+        <v>128</v>
       </c>
     </row>
     <row r="26" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>26</v>
+        <v>79</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>107</v>
+        <v>160</v>
       </c>
     </row>
     <row r="29" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>27</v>
+        <v>78</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>108</v>
+        <v>159</v>
       </c>
     </row>
     <row r="30" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>28</v>
+        <v>80</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
     </row>
     <row r="32" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>31</v>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="51" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>112</v>
+        <v>97</v>
       </c>
     </row>
     <row r="34" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>113</v>
+        <v>83</v>
       </c>
     </row>
     <row r="35" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>33</v>
+        <v>0</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>114</v>
+        <v>81</v>
       </c>
     </row>
     <row r="36" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>34</v>
+        <v>1</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>115</v>
+        <v>82</v>
       </c>
     </row>
     <row r="37" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>35</v>
+        <v>59</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>116</v>
+        <v>140</v>
       </c>
     </row>
     <row r="38" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>36</v>
+        <v>60</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
-        <v>37</v>
+        <v>141</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
+        <v>50</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>118</v>
+        <v>131</v>
       </c>
     </row>
     <row r="40" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>38</v>
+        <v>61</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>119</v>
+        <v>142</v>
       </c>
     </row>
     <row r="41" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>39</v>
+        <v>62</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
-        <v>40</v>
+        <v>143</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="4" t="s">
+        <v>63</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="6" t="s">
-        <v>41</v>
+        <v>144</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
+        <v>64</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>122</v>
+        <v>145</v>
       </c>
     </row>
     <row r="44" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>42</v>
+        <v>65</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="2" t="s">
-        <v>43</v>
+        <v>146</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
+        <v>5</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>124</v>
+        <v>86</v>
       </c>
     </row>
     <row r="46" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>44</v>
+        <v>72</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>125</v>
+        <v>153</v>
       </c>
     </row>
     <row r="47" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>45</v>
+        <v>68</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>126</v>
+        <v>149</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>127</v>
+        <v>150</v>
       </c>
     </row>
     <row r="49" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>47</v>
+        <v>73</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>128</v>
+        <v>154</v>
       </c>
     </row>
     <row r="50" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>48</v>
+        <v>70</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="4" t="s">
-        <v>49</v>
+        <v>151</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
+        <v>74</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="4" t="s">
-        <v>50</v>
+        <v>155</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
+        <v>75</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="2" t="s">
-        <v>52</v>
+        <v>152</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="4" t="s">
+        <v>66</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="2" t="s">
-        <v>53</v>
+        <v>147</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="4" t="s">
+        <v>67</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="2" t="s">
-        <v>54</v>
+        <v>148</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>135</v>
+        <v>99</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>137</v>
+        <v>110</v>
       </c>
     </row>
     <row r="59" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>58</v>
+        <v>32</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>139</v>
+        <v>113</v>
       </c>
     </row>
     <row r="61" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>59</v>
+        <v>76</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="4" t="s">
-        <v>63</v>
+        <v>137</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
+        <v>57</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="4" t="s">
-        <v>64</v>
+        <v>138</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>65</v>
+        <v>13</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="2" t="s">
-        <v>66</v>
+        <v>94</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A68" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="4" t="s">
-        <v>67</v>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>148</v>
+        <v>119</v>
       </c>
     </row>
     <row r="70" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
     </row>
     <row r="72" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="2" t="s">
-        <v>72</v>
+        <v>139</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" s="4" t="s">
+        <v>49</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="2" t="s">
-        <v>73</v>
+        <v>130</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" s="4" t="s">
+        <v>4</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>154</v>
+        <v>85</v>
       </c>
     </row>
     <row r="76" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
-        <v>74</v>
+        <v>30</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>75</v>
+        <v>34</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>76</v>
+        <v>51</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
-        <v>77</v>
+        <v>52</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>158</v>
+        <v>133</v>
       </c>
     </row>
     <row r="80" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
-        <v>78</v>
+        <v>43</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>159</v>
+        <v>124</v>
       </c>
     </row>
     <row r="81" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
-        <v>79</v>
+        <v>44</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>160</v>
+        <v>125</v>
       </c>
     </row>
     <row r="82" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
-        <v>80</v>
+        <v>45</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>161</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>

</xml_diff>